<commit_message>
AFDP-520 - Case - Move Case Plugin code into ACM core - create case file folder in Alfresco
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>RuleSet</t>
   </si>
@@ -100,7 +100,16 @@
     <t>ecmFolderId == null</t>
   </si>
   <si>
-    <t>setEcmFolderPath, '/Sites/acm/documentLibrary/CaseFiles/' + dateFormat('yyyyMMdd') + '_' + $caseFile.getId()</t>
+    <t>setEcmFolderPath, '/Sites/acm/documentLibrary/Case Files/' + dateFormat('yyyyMMdd') + '_' + $caseFile.getId()</t>
+  </si>
+  <si>
+    <t>Set Case Status</t>
+  </si>
+  <si>
+    <t>status == null</t>
+  </si>
+  <si>
+    <t>setStatus, 'DRAFT'</t>
   </si>
 </sst>
 </file>
@@ -466,7 +475,7 @@
   <dimension ref="A2:D27"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D7" activeCellId="0" pane="topLeft" sqref="D7"/>
+      <selection activeCell="D16" activeCellId="0" pane="topLeft" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -624,9 +633,15 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
       <c r="A17" s="1"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
+      <c r="B17" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="18">
       <c r="A18" s="1"/>

</xml_diff>

<commit_message>
AFDP-157 - Add Access Control List to SOLR documents - apply assignment and data access control rules to case files
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="274" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="134" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
   <si>
     <t>RuleSet</t>
   </si>
@@ -131,15 +131,6 @@
   </si>
   <si>
     <t>setPriority,'Medium'</t>
-  </si>
-  <si>
-    <t>Set Assignee</t>
-  </si>
-  <si>
-    <t>assignee == null</t>
-  </si>
-  <si>
-    <t>setAssignee, 'ann-acm'</t>
   </si>
   <si>
     <t>Set Due Date</t>
@@ -511,10 +502,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:D29"/>
+  <dimension ref="A2:D65536"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D20" activeCellId="0" pane="topLeft" sqref="D20"/>
+      <selection activeCell="C22" activeCellId="0" pane="topLeft" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -727,17 +718,11 @@
         <v>37</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.7" outlineLevel="0" r="22">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
       <c r="A22" s="1"/>
-      <c r="B22" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>40</v>
-      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
       <c r="A23" s="1"/>
@@ -775,12 +760,7 @@
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
-      <c r="A29" s="1"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
AFDP-559 - SOLR enhancements - batch reindex fixes:  ensure DAC filters work with reindexing; update Drools version; apply a stable sort order to the batch reindex SOLR query
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
@@ -22,7 +22,7 @@
     <t>RuleSet</t>
   </si>
   <si>
-    <t>Save Complaint Rules</t>
+    <t>Save Case File Rules</t>
   </si>
   <si>
     <t>Import</t>
@@ -67,7 +67,7 @@
     <t>true</t>
   </si>
   <si>
-    <t>RuleTable Save Case Rules</t>
+    <t>RuleTable Save Case File Rules</t>
   </si>
   <si>
     <t>CONDITION</t>
@@ -504,8 +504,8 @@
   </sheetPr>
   <dimension ref="A2:D65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A4" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C22" activeCellId="0" pane="topLeft" sqref="C22"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C13" activeCellId="0" pane="topLeft" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -518,7 +518,7 @@
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.70918367346939"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -608,7 +608,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">

</xml_diff>

<commit_message>
AFDP-892 - Store container folder IDs in a single shared table, not in columns in the container's table - convert CaseFile module to use AcmContainerFolder
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="134" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="111" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -109,7 +109,7 @@
     <t>Assign Alfresco Folder</t>
   </si>
   <si>
-    <t>ecmFolderId == null</t>
+    <t>containerFolder.cmisFolderId == null</t>
   </si>
   <si>
     <t>setEcmFolderPath, '/Sites/acm/documentLibrary/Case Files/' + dateFormat('yyyyMMdd') + '_' + $caseFile.getId()</t>
@@ -136,7 +136,7 @@
     <t>Set Due Date</t>
   </si>
   <si>
-    <t>DueDate == null</t>
+    <t>dueDate == null</t>
   </si>
   <si>
     <t>setDueDate, addDays(180)</t>
@@ -504,8 +504,8 @@
   </sheetPr>
   <dimension ref="A2:D65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C13" activeCellId="0" pane="topLeft" sqref="C13"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D20" activeCellId="0" pane="topLeft" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -670,7 +670,7 @@
         <v>25</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="18">
       <c r="A18" s="1"/>
       <c r="B18" s="17" t="s">
         <v>26</v>
@@ -706,7 +706,7 @@
         <v>34</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.7" outlineLevel="0" r="21">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="21">
       <c r="A21" s="1"/>
       <c r="B21" s="17" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
AFDP-894 - Update all code to upload new files to populate ACM_FILE and ACM_FILE_REVISION tables - JPA Entity and service changes - all file uploads seem to work now
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
   <si>
     <t>RuleSet</t>
   </si>
@@ -46,10 +46,26 @@
     <t>java.util.Calendar</t>
   </si>
   <si>
+    <t>org.springframework.expression.EvaluationContext</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.Expression</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.ExpressionParser</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.spel.standard.SpelExpressionParser</t>
+  </si>
+  <si>
+    <t>org.springframework.expression.spel.support.StandardEvaluationContext</t>
+  </si>
+  <si>
     <t>Functions</t>
   </si>
   <si>
-    <t>function String dateFormat(String fmt)
+    <r>
+      <t xml:space="preserve">function String dateFormat(String fmt)
 {
   return LocalDate.now().toString(DateTimeFormat.forPattern(fmt));
 }
@@ -58,7 +74,25 @@
   Calendar cal = Calendar.getInstance();
   cal.add(Calendar.DAY_OF_YEAR, days);
   return cal.getTime();
+}
+function Boolean evalSpring(String expression, Object obj)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{
+    ExpressionParser ep = new SpelExpressionParser();
+    Expression exp = ep.parseExpression(expression);
+    EvaluationContext ec = new StandardEvaluationContext();
+    Boolean evaluated = exp.getValue(ec, obj, Boolean.class);
+    return evaluated;
 }</t>
+    </r>
   </si>
   <si>
     <t>Sequential</t>
@@ -79,7 +113,7 @@
     <t>$caseFile: CaseFile</t>
   </si>
   <si>
-    <t>$param == true</t>
+    <t>eval(evalSpring("$param", $caseFile))</t>
   </si>
   <si>
     <t>$caseFile.$1($2);</t>
@@ -109,7 +143,7 @@
     <t>Assign Alfresco Folder</t>
   </si>
   <si>
-    <t>containerFolder.cmisFolderId == null</t>
+    <t>container?.folder?.cmisFolderId == null</t>
   </si>
   <si>
     <t>setEcmFolderPath, '/Sites/acm/documentLibrary/Case Files/' + dateFormat('yyyyMMdd') + '_' + $caseFile.getId()</t>
@@ -149,7 +183,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -178,6 +212,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -393,7 +433,7 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="4" fontId="0" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="4" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -504,8 +544,8 @@
   </sheetPr>
   <dimension ref="A2:D65536"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D20" activeCellId="0" pane="topLeft" sqref="D20"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C14" activeCellId="0" pane="topLeft" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -588,165 +628,185 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="121" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>11</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
+      <c r="C12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
+        <v>2</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="247.75" outlineLevel="0" r="14">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="10"/>
+        <v>14</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="12" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="34.05" outlineLevel="0" r="16">
-      <c r="A16" s="13" t="s">
+      <c r="D17" s="2"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="D18" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="17">
-      <c r="A17" s="1"/>
-      <c r="B17" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="18">
-      <c r="A18" s="1"/>
-      <c r="B18" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>28</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
       <c r="A19" s="1"/>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="1"/>
+      <c r="C19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="10"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="34.05" outlineLevel="0" r="21">
+      <c r="A21" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="22">
+      <c r="A22" s="1"/>
+      <c r="B22" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="D22" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="17" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+      <c r="A23" s="1"/>
+      <c r="B23" s="17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.7" outlineLevel="0" r="20">
-      <c r="A20" s="1"/>
-      <c r="B20" s="17" t="s">
+      <c r="C23" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="17" t="s">
+      <c r="D23" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="21">
-      <c r="A21" s="1"/>
-      <c r="B21" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
-      <c r="A22" s="1"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">
-      <c r="A23" s="1"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
       <c r="A24" s="1"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="25">
+      <c r="B24" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.7" outlineLevel="0" r="25">
       <c r="A25" s="1"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="26">
+      <c r="B25" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="26">
       <c r="A26" s="1"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
+      <c r="B26" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="27">
       <c r="A27" s="1"/>
@@ -759,6 +819,36 @@
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
+      <c r="A29" s="1"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="30">
+      <c r="A30" s="1"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="31">
+      <c r="A31" s="1"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="32">
+      <c r="A32" s="1"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="33">
+      <c r="A33" s="1"/>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
   </sheetData>

</xml_diff>

<commit_message>
AFDP-1005: eBrief Form - New Changes
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riste.tutureski\Desktop\AFDP-1056\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="111" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="111"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t>RuleSet</t>
   </si>
@@ -85,7 +89,7 @@
         <rFont val="Calibri"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">{
+      <t>{
     ExpressionParser ep = new SpelExpressionParser();
     Expression exp = ep.parseExpression(expression);
     EvaluationContext ec = new StandardEvaluationContext();
@@ -175,36 +179,27 @@
   <si>
     <t>setDueDate, addDays(180)</t>
   </si>
+  <si>
+    <t>Set Title as Case Number if null</t>
+  </si>
+  <si>
+    <t>title == null</t>
+  </si>
+  <si>
+    <t>setTitle, $caseFile.getCaseNumber()</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
@@ -271,209 +266,221 @@
     </fill>
   </fills>
   <borders count="13">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="medium"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="medium"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="thin"/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="medium"/>
-      <right style="medium"/>
-      <top style="thin"/>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalDown="false" diagonalUp="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="3" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="4" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="10" fillId="4" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="5" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="6" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="7" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="8" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="11" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="12" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -532,33 +539,307 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A2:D65536"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D33"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A7" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C14" activeCellId="0" pane="topLeft" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4183673469388"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2908163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.1428571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="100.423469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.719387755102"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.70918367346939"/>
+    <col min="1" max="1" width="19.42578125"/>
+    <col min="2" max="2" width="24.28515625"/>
+    <col min="3" max="3" width="50.140625"/>
+    <col min="4" max="4" width="100.42578125"/>
+    <col min="5" max="5" width="27.7109375"/>
+    <col min="6" max="1025" width="8.7109375"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
@@ -568,7 +849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="4" t="s">
@@ -578,7 +859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="4" t="s">
@@ -588,7 +869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="4" t="s">
@@ -598,7 +879,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="4" t="s">
@@ -608,7 +889,7 @@
         <v>6</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.7" outlineLevel="0" r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="4" t="s">
@@ -618,7 +899,7 @@
         <v>7</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.7" outlineLevel="0" r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="4" t="s">
@@ -628,7 +909,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="4" t="s">
@@ -638,7 +919,7 @@
         <v>9</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="4" t="s">
@@ -648,7 +929,7 @@
         <v>10</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
@@ -658,7 +939,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
@@ -668,7 +949,7 @@
         <v>12</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
@@ -678,7 +959,7 @@
         <v>13</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="247.75" outlineLevel="0" r="14">
+    <row r="14" spans="1:4" ht="330" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -688,7 +969,7 @@
         <v>15</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="8" t="s">
@@ -698,7 +979,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
@@ -706,7 +987,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="4" t="s">
@@ -716,7 +997,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="4" t="s">
@@ -724,7 +1005,7 @@
       </c>
       <c r="D19" s="10"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="11" t="s">
@@ -734,7 +1015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="34.05" outlineLevel="0" r="21">
+    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="13" t="s">
         <v>24</v>
       </c>
@@ -748,7 +1029,7 @@
         <v>27</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="14.25" outlineLevel="0" r="22">
+    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="17" t="s">
         <v>28</v>
@@ -760,7 +1041,7 @@
         <v>30</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="23">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="17" t="s">
         <v>31</v>
@@ -772,7 +1053,7 @@
         <v>33</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="24">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
         <v>34</v>
@@ -784,7 +1065,7 @@
         <v>36</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.7" outlineLevel="0" r="25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
         <v>37</v>
@@ -796,7 +1077,7 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.8" outlineLevel="0" r="26">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
         <v>40</v>
@@ -808,108 +1089,88 @@
         <v>42</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="27">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="28">
+      <c r="B27" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="29">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="30">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="31">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="32">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="17"/>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="33">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="17"/>
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1048576"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.70918367346939"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.70918367346939"/>
+    <col min="1" max="1025" width="8.7109375"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AFDP-1063: Brief Title and File Name
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riste.tutureski\Desktop\AFDP-1056\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riste.tutureski\.acm\rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -186,7 +186,7 @@
     <t>title == null</t>
   </si>
   <si>
-    <t>setTitle, $caseFile.getCaseNumber()</t>
+    <t>setTitle, 'Brief #' + $caseFile.getCaseNumber()</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
AFDP-1080: Changing Brief title format
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="48">
   <si>
     <t>RuleSet</t>
   </si>
@@ -68,37 +68,6 @@
     <t>Functions</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">function String dateFormat(String fmt)
-{
-  return LocalDate.now().toString(DateTimeFormat.forPattern(fmt));
-}
-function Date addDays(int days)
-{
-  Calendar cal = Calendar.getInstance();
-  cal.add(Calendar.DAY_OF_YEAR, days);
-  return cal.getTime();
-}
-function Boolean evalSpring(String expression, Object obj)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>{
-    ExpressionParser ep = new SpelExpressionParser();
-    Expression exp = ep.parseExpression(expression);
-    EvaluationContext ec = new StandardEvaluationContext();
-    Boolean evaluated = exp.getValue(ec, obj, Boolean.class);
-    return evaluated;
-}</t>
-    </r>
-  </si>
-  <si>
     <t>Sequential</t>
   </si>
   <si>
@@ -183,10 +152,63 @@
     <t>Set Title as Case Number if null</t>
   </si>
   <si>
-    <t>title == null</t>
-  </si>
-  <si>
-    <t>setTitle, 'Brief #' + $caseFile.getCaseNumber()</t>
+    <t>com.armedia.acm.plugins.person.model.Person</t>
+  </si>
+  <si>
+    <t>com.armedia.acm.plugins.person.model.PersonAssociation</t>
+  </si>
+  <si>
+    <t>setTitle, createTitle($caseFile)</t>
+  </si>
+  <si>
+    <t>function String dateFormat(String fmt)
+    {
+      return LocalDate.now().toString(DateTimeFormat.forPattern(fmt));
+    }
+    function Date addDays(int days)
+    {
+      Calendar cal = Calendar.getInstance();
+      cal.add(Calendar.DAY_OF_YEAR, days);
+      return cal.getTime();
+    }
+    function Boolean evalSpring(String expression, Object obj)
+    {
+        ExpressionParser ep = new SpelExpressionParser();
+        Expression exp = ep.parseExpression(expression);
+        EvaluationContext ec = new StandardEvaluationContext();
+        Boolean evaluated = exp.getValue(ec, obj, Boolean.class);
+        return evaluated;
+    }
+    function String createTitle(CaseFile caseFile)
+    {
+        String lastName = "";
+        String caseNumber = "";
+        if (caseFile != null)
+        {
+            if (caseFile.getPersonAssociations() != null)
+            {
+                for (PersonAssociation pa : caseFile.getPersonAssociations())
+                {
+                   if ("Defendant".equalsIgnoreCase(pa.getPersonType()))
+                   {
+                      if (pa.getPerson() != null &amp;&amp; pa.getPerson().getFamilyName() != null)
+                      {
+                         lastName = pa.getPerson().getFamilyName();
+                         break;
+                      }
+                   }
+               }
+           }
+           if (caseFile.getCaseNumber() != null)
+           {
+              caseNumber = caseFile.getCaseNumber();
+           }
+        }
+        return lastName + "_" + caseNumber;
+    }</t>
+  </si>
+  <si>
+    <t>title == null || title != null</t>
   </si>
 </sst>
 </file>
@@ -447,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -475,6 +497,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,10 +846,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D33"/>
+  <dimension ref="A2:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="B17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,163 +978,171 @@
       <c r="C13" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="330" x14ac:dyDescent="0.25">
+      <c r="D13" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>15</v>
+        <v>2</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-      <c r="C15" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>17</v>
+      <c r="C15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>20</v>
+      <c r="C17" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="10"/>
+      <c r="C19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="12" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="B23" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="C23" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="D23" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>35</v>
+        <v>27</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>28</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>38</v>
+        <v>30</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>31</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="17" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="17" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
+      <c r="B28" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
+      <c r="B29" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
@@ -1137,9 +1168,21 @@
       <c r="C33" s="17"/>
       <c r="D33" s="17"/>
     </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="17"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="17"/>
+      <c r="D35" s="17"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
AFDP-1080: Changing Brief title format - Set default name to 'Brief'
</commit_message>
<xml_diff>
--- a/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
+++ b/acm-plugins/acm-default-plugins/acm-case-file-plugin/src/main/resources/rules/drools-case-file-rules.xlsx
@@ -161,6 +161,9 @@
     <t>setTitle, createTitle($caseFile)</t>
   </si>
   <si>
+    <t>title == null || title != null</t>
+  </si>
+  <si>
     <t>function String dateFormat(String fmt)
     {
       return LocalDate.now().toString(DateTimeFormat.forPattern(fmt));
@@ -181,7 +184,7 @@
     }
     function String createTitle(CaseFile caseFile)
     {
-        String lastName = "";
+        String lastName = "Brief";
         String caseNumber = "";
         if (caseFile != null)
         {
@@ -206,9 +209,6 @@
         }
         return lastName + "_" + caseNumber;
     }</t>
-  </si>
-  <si>
-    <t>title == null || title != null</t>
   </si>
 </sst>
 </file>
@@ -848,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="B14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,7 +1009,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1138,7 +1138,7 @@
         <v>42</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>45</v>

</xml_diff>